<commit_message>
updated mac version to 0.0.0.0.12
</commit_message>
<xml_diff>
--- a/examples/rules.xlsx
+++ b/examples/rules.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jww/Developer/python/terraformer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C144A47-2836-E049-9A7F-7E29732C338B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66A5AEFC-24A9-F348-814B-E4CE08027FDD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43100" yWindow="-16260" windowWidth="25600" windowHeight="14680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="acls" sheetId="51" r:id="rId1"/>
-    <sheet name="securitygroups" sheetId="52" r:id="rId2"/>
+    <sheet name="aclrules" sheetId="51" r:id="rId1"/>
+    <sheet name="sgheaders" sheetId="53" r:id="rId2"/>
+    <sheet name="sgrules" sheetId="52" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="30">
   <si>
     <t>*name</t>
   </si>
@@ -46,9 +47,6 @@
     <t>protocol</t>
   </si>
   <si>
-    <t>iacl1rule100</t>
-  </si>
-  <si>
     <t>allow</t>
   </si>
   <si>
@@ -61,15 +59,9 @@
     <t>tcp:80:80</t>
   </si>
   <si>
-    <t>iacl1rule200</t>
-  </si>
-  <si>
     <t>udp:805:807</t>
   </si>
   <si>
-    <t>eacl1rule100</t>
-  </si>
-  <si>
     <t>outbound</t>
   </si>
   <si>
@@ -79,28 +71,52 @@
     <t>ip_version</t>
   </si>
   <si>
-    <t>isg1rule100</t>
-  </si>
-  <si>
     <t>127.0.0.1</t>
   </si>
   <si>
-    <t>esg1rule200</t>
-  </si>
-  <si>
-    <t>isg2rule100</t>
-  </si>
-  <si>
-    <t>esg2rule200</t>
-  </si>
-  <si>
-    <t>#sg1:vpc1</t>
-  </si>
-  <si>
-    <t>#sg2:vpc1</t>
-  </si>
-  <si>
-    <t>#acl1</t>
+    <t>sg1</t>
+  </si>
+  <si>
+    <t>sg2</t>
+  </si>
+  <si>
+    <t>*vpc</t>
+  </si>
+  <si>
+    <t>resource_group</t>
+  </si>
+  <si>
+    <t>vpc1</t>
+  </si>
+  <si>
+    <t>*acl</t>
+  </si>
+  <si>
+    <t>acl1</t>
+  </si>
+  <si>
+    <t>*group</t>
+  </si>
+  <si>
+    <t>insg1rule100</t>
+  </si>
+  <si>
+    <t>outsg1rule200</t>
+  </si>
+  <si>
+    <t>insg2rule100</t>
+  </si>
+  <si>
+    <t>outsg2rule200</t>
+  </si>
+  <si>
+    <t>inacl1rule100</t>
+  </si>
+  <si>
+    <t>inacl1rule200</t>
+  </si>
+  <si>
+    <t>outacl1rule100</t>
   </si>
 </sst>
 </file>
@@ -158,7 +174,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -169,11 +185,18 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="22">
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -229,6 +252,45 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -259,25 +321,39 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8524F582-25D9-D64B-A9C7-4FF4A27248B3}" name="Table1" displayName="Table1" ref="A1:F5" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
-  <autoFilter ref="A1:F5" xr:uid="{00881A37-2AAB-7345-9099-83242FC8EDEA}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{36FEA897-58B8-8244-BBD2-F934FDEC8E9A}" name="*name" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{F12A4B82-233E-A440-B918-86C5E4C82FD9}" name="*action" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{568185F1-B557-2C49-B724-A15618F6D5DE}" name="*source" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{F5A78E34-0750-6E4E-BE76-F9B327F65E12}" name="*destination" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{83261B25-C691-8D45-8989-863A46F2510F}" name="*direction" dataDxfId="8"/>
-    <tableColumn id="11" xr3:uid="{DA919A14-BC6E-5547-A993-1B7855521094}" name="protocol" dataDxfId="7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8524F582-25D9-D64B-A9C7-4FF4A27248B3}" name="Table1" displayName="Table1" ref="A1:G4" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+  <autoFilter ref="A1:G4" xr:uid="{00881A37-2AAB-7345-9099-83242FC8EDEA}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{36FEA897-58B8-8244-BBD2-F934FDEC8E9A}" name="*name" dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{C499C2EF-3238-4B4A-8017-492B9A1A77FF}" name="*acl" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{F12A4B82-233E-A440-B918-86C5E4C82FD9}" name="*action" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{568185F1-B557-2C49-B724-A15618F6D5DE}" name="*source" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{F5A78E34-0750-6E4E-BE76-F9B327F65E12}" name="*destination" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{83261B25-C691-8D45-8989-863A46F2510F}" name="*direction" dataDxfId="14"/>
+    <tableColumn id="11" xr3:uid="{DA919A14-BC6E-5547-A993-1B7855521094}" name="protocol" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{11008CC8-5C85-3B48-82BD-CD830AD3D6DF}" name="Table18" displayName="Table18" ref="A1:E8" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A1:E8" xr:uid="{EF08DB4E-0002-F047-8599-404D4BBF8940}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{203C77A6-285B-124C-AF24-A3511F6244F7}" name="*name" dataDxfId="4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{83144CBC-65AD-804B-B36C-148A65E84D16}" name="Table184" displayName="Table184" ref="A1:C3" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A1:C3" xr:uid="{EF08DB4E-0002-F047-8599-404D4BBF8940}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{A724ADCC-F039-0D45-9937-58B50BC5715E}" name="*name" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{B9D7A6DC-911D-B749-AE7A-2DC2D907D356}" name="*vpc" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{CE9B4557-50B5-2A4A-AA03-F9F781F4F349}" name="resource_group" dataDxfId="8"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{11008CC8-5C85-3B48-82BD-CD830AD3D6DF}" name="Table18" displayName="Table18" ref="A1:F6" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F6" xr:uid="{EF08DB4E-0002-F047-8599-404D4BBF8940}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{203C77A6-285B-124C-AF24-A3511F6244F7}" name="*name" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{2F8C3C4B-0E49-4A4D-AC20-F814AA26DD74}" name="*group" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{42DAC7A2-384A-144A-9BDC-F241D22F7F74}" name="*direction" dataDxfId="3"/>
     <tableColumn id="3" xr3:uid="{41DCA0FA-BF94-6343-BF46-01D165299C09}" name="*remote" dataDxfId="2"/>
     <tableColumn id="4" xr3:uid="{15B7721A-4EE3-9847-9C27-38416048A9AE}" name="ip_version" dataDxfId="1"/>
@@ -550,99 +626,101 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FB3C17B-7688-8D45-9DEE-F9650DD6901F}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="B3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="1"/>
+      <c r="G4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -653,8 +731,8 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF3D3370-44D8-0A42-8C42-E9D4E75B0DB2}">
-  <dimension ref="A1:E9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F29E99F-EAC6-EF42-BBDE-1489EAD1BB17}">
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -665,105 +743,156 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="1"/>
+        <v>15</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF3D3370-44D8-0A42-8C42-E9D4E75B0DB2}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1" t="s">
         <v>9</v>
       </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="C3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="1" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+        <v>26</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>